<commit_message>
fix duplicate family id on family sheet
</commit_message>
<xml_diff>
--- a/lib/devdata/ajl.xlsx
+++ b/lib/devdata/ajl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MEASBona/oscar-web/lib/devdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA86B7E-53E4-224B-BFB6-04759F67216C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591F42C8-219D-A040-BDAF-67FA13D74056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="4" r:id="rId1"/>
@@ -2267,9 +2267,9 @@
   </sheetPr>
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView zoomScale="174" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2671,9 +2671,7 @@
       <c r="A13" s="51" t="s">
         <v>388</v>
       </c>
-      <c r="B13" s="18">
-        <v>67</v>
-      </c>
+      <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
         <v>58</v>
       </c>
@@ -4416,7 +4414,7 @@
   </sheetPr>
   <dimension ref="A1:AP1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AJ16"/>
     </sheetView>

</xml_diff>